<commit_message>
renamed directories for consistency
same length event and source names
</commit_message>
<xml_diff>
--- a/Letter.xlsx
+++ b/Letter.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-34020" yWindow="2360" windowWidth="28800" windowHeight="17460" tabRatio="500"/>
+    <workbookView xWindow="2800" yWindow="460" windowWidth="28800" windowHeight="17460" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
   <si>
     <t>AJC</t>
   </si>
@@ -57,9 +57,6 @@
   </si>
   <si>
     <t>VT</t>
-  </si>
-  <si>
-    <t>WSM</t>
   </si>
   <si>
     <t>NIU</t>
@@ -115,7 +112,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="15">
     <border>
       <left/>
       <right/>
@@ -138,11 +135,186 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -150,6 +322,28 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="14" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -427,15 +621,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G25"/>
+  <dimension ref="A1:G24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L13" sqref="L13"/>
+    <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="J8" sqref="J8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:7" s="1" customFormat="1" ht="36" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" s="1" customFormat="1" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="24"/>
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -455,64 +650,64 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="36" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
+    <row r="2" spans="1:7" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="2"/>
-      <c r="C2" s="2"/>
-      <c r="D2" s="2"/>
-      <c r="E2" s="2"/>
-      <c r="F2" s="2"/>
-      <c r="G2" s="2"/>
+      <c r="B2" s="8"/>
+      <c r="C2" s="8"/>
+      <c r="D2" s="8"/>
+      <c r="E2" s="8"/>
+      <c r="F2" s="8"/>
+      <c r="G2" s="9"/>
     </row>
     <row r="3" spans="1:7" ht="36" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>16</v>
-      </c>
-      <c r="B3" s="4"/>
-      <c r="C3" s="4"/>
-      <c r="D3" s="4"/>
-      <c r="E3" s="4"/>
-      <c r="F3" s="4"/>
-      <c r="G3" s="2"/>
-    </row>
-    <row r="4" spans="1:7" ht="36" customHeight="1" x14ac:dyDescent="0.2">
+        <v>15</v>
+      </c>
+      <c r="B3" s="5"/>
+      <c r="C3" s="5"/>
+      <c r="D3" s="5"/>
+      <c r="E3" s="5"/>
+      <c r="F3" s="5"/>
+      <c r="G3" s="6"/>
+    </row>
+    <row r="4" spans="1:7" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>14</v>
-      </c>
-      <c r="B4" s="4"/>
-      <c r="C4" s="4"/>
-      <c r="D4" s="4"/>
-      <c r="E4" s="2"/>
-      <c r="F4" s="3"/>
-      <c r="G4" s="3"/>
-    </row>
-    <row r="5" spans="1:7" ht="36" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
+        <v>13</v>
+      </c>
+      <c r="B4" s="10"/>
+      <c r="C4" s="10"/>
+      <c r="D4" s="10"/>
+      <c r="E4" s="11"/>
+      <c r="F4" s="12"/>
+      <c r="G4" s="12"/>
+    </row>
+    <row r="5" spans="1:7" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="B5" s="2"/>
-      <c r="C5" s="2"/>
-      <c r="D5" s="3"/>
-      <c r="E5" s="2"/>
-      <c r="F5" s="2"/>
-      <c r="G5" s="2"/>
+      <c r="B5" s="8"/>
+      <c r="C5" s="8"/>
+      <c r="D5" s="14"/>
+      <c r="E5" s="8"/>
+      <c r="F5" s="8"/>
+      <c r="G5" s="9"/>
     </row>
     <row r="6" spans="1:7" ht="36" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>8</v>
       </c>
-      <c r="B6" s="2"/>
-      <c r="C6" s="3"/>
-      <c r="D6" s="3"/>
-      <c r="E6" s="3"/>
-      <c r="F6" s="3"/>
-      <c r="G6" s="3"/>
+      <c r="B6" s="6"/>
+      <c r="C6" s="13"/>
+      <c r="D6" s="13"/>
+      <c r="E6" s="13"/>
+      <c r="F6" s="13"/>
+      <c r="G6" s="13"/>
     </row>
     <row r="7" spans="1:7" ht="36" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B7" s="4"/>
       <c r="C7" s="2"/>
@@ -523,7 +718,7 @@
     </row>
     <row r="8" spans="1:7" ht="36" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B8" s="4"/>
       <c r="C8" s="4"/>
@@ -532,30 +727,30 @@
       <c r="F8" s="3"/>
       <c r="G8" s="2"/>
     </row>
-    <row r="9" spans="1:7" ht="36" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:7" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>13</v>
-      </c>
-      <c r="B9" s="4"/>
-      <c r="C9" s="4"/>
-      <c r="D9" s="2"/>
-      <c r="E9" s="3"/>
-      <c r="F9" s="3"/>
-      <c r="G9" s="2"/>
+        <v>12</v>
+      </c>
+      <c r="B9" s="10"/>
+      <c r="C9" s="10"/>
+      <c r="D9" s="11"/>
+      <c r="E9" s="12"/>
+      <c r="F9" s="12"/>
+      <c r="G9" s="11"/>
     </row>
     <row r="10" spans="1:7" ht="36" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" t="s">
-        <v>15</v>
-      </c>
-      <c r="B10" s="2"/>
-      <c r="C10" s="2"/>
-      <c r="D10" s="2"/>
-      <c r="E10" s="2"/>
-      <c r="F10" s="2"/>
-      <c r="G10" s="2"/>
+      <c r="A10" s="15" t="s">
+        <v>14</v>
+      </c>
+      <c r="B10" s="16"/>
+      <c r="C10" s="16"/>
+      <c r="D10" s="16"/>
+      <c r="E10" s="16"/>
+      <c r="F10" s="16"/>
+      <c r="G10" s="17"/>
     </row>
     <row r="11" spans="1:7" ht="36" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" t="s">
+      <c r="A11" s="18" t="s">
         <v>9</v>
       </c>
       <c r="B11" s="2"/>
@@ -563,31 +758,23 @@
       <c r="D11" s="2"/>
       <c r="E11" s="2"/>
       <c r="F11" s="2"/>
-      <c r="G11" s="2"/>
-    </row>
-    <row r="12" spans="1:7" ht="36" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" t="s">
+      <c r="G11" s="19"/>
+    </row>
+    <row r="12" spans="1:7" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="20" t="s">
         <v>10</v>
       </c>
-      <c r="B12" s="2"/>
-      <c r="C12" s="2"/>
-      <c r="D12" s="2"/>
-      <c r="E12" s="2"/>
-      <c r="F12" s="2"/>
-      <c r="G12" s="2"/>
-    </row>
-    <row r="13" spans="1:7" ht="36" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" t="s">
-        <v>11</v>
-      </c>
-      <c r="B13" s="3"/>
-      <c r="C13" s="2"/>
-      <c r="D13" s="3"/>
-      <c r="E13" s="3"/>
-      <c r="F13" s="3"/>
-      <c r="G13" s="3"/>
-    </row>
-    <row r="14" spans="1:7" ht="36" customHeight="1" x14ac:dyDescent="0.2"/>
+      <c r="B12" s="21"/>
+      <c r="C12" s="21"/>
+      <c r="D12" s="21"/>
+      <c r="E12" s="21"/>
+      <c r="F12" s="21"/>
+      <c r="G12" s="22"/>
+    </row>
+    <row r="13" spans="1:7" ht="36" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="14" spans="1:7" ht="36" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A14" s="23"/>
+    </row>
     <row r="15" spans="1:7" ht="36" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="16" spans="1:7" ht="36" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="17" ht="36" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -598,7 +785,6 @@
     <row r="22" ht="36" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="23" ht="36" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="24" ht="36" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="25" ht="36" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>